<commit_message>
initial work on figures completed
</commit_message>
<xml_diff>
--- a/2022CCSurvey_1.xlsx
+++ b/2022CCSurvey_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/kolby_grint_usda_gov/Documents/Documents/R Vizualizations and Data/Chippewa-County-Cover-Crop-Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49D5DB15-F316-4AFA-A66D-21BBF3D84081}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6153BD4-DDF6-4855-9B63-F51C42F3EDB2}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11325" xr2:uid="{3ABCB6C5-5AC4-4763-96A0-86D19504B3A4}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{3ABCB6C5-5AC4-4763-96A0-86D19504B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="169">
   <si>
     <t>respondent</t>
   </si>
@@ -42,12 +42,6 @@
     <t>township</t>
   </si>
   <si>
-    <t>cropland_acres</t>
-  </si>
-  <si>
-    <t>cc_acres</t>
-  </si>
-  <si>
     <t>prior_crops</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>cc_plant</t>
   </si>
   <si>
-    <t>Conventional drill</t>
-  </si>
-  <si>
     <t>tillage</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>lastplant_date</t>
   </si>
   <si>
-    <t>spinner broadcast only</t>
-  </si>
-  <si>
     <t>bin run</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>cover only then plant</t>
   </si>
   <si>
-    <t>cover only, then plant</t>
-  </si>
-  <si>
     <t>plant brown</t>
   </si>
   <si>
@@ -234,18 +219,12 @@
     <t>time to plant cover crops</t>
   </si>
   <si>
-    <t>convential drill</t>
-  </si>
-  <si>
     <t>late harvesst</t>
   </si>
   <si>
     <t>Colburn</t>
   </si>
   <si>
-    <t>air-flow broadcast only</t>
-  </si>
-  <si>
     <t>Eagle Point</t>
   </si>
   <si>
@@ -267,9 +246,6 @@
     <t>drill plugging from bin run seed</t>
   </si>
   <si>
-    <t>common variety from supplier</t>
-  </si>
-  <si>
     <t>Hallie,Lafayette</t>
   </si>
   <si>
@@ -279,9 +255,6 @@
     <t>no-till,shallow vertical</t>
   </si>
   <si>
-    <t>no-till drill, air-flow broadcast + shallow till</t>
-  </si>
-  <si>
     <t>winter rye, winter wheat</t>
   </si>
   <si>
@@ -387,9 +360,6 @@
     <t>winter rye,oats,clover,peas,buckwheat,turnips</t>
   </si>
   <si>
-    <t>no-till drill,spinner broadcast only,fly-on</t>
-  </si>
-  <si>
     <t>bin run,common variety</t>
   </si>
   <si>
@@ -484,6 +454,93 @@
   </si>
   <si>
     <t>100,100</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>soil conservation,nutrient management</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>soil conservation,groundwater quality,curiosity,incentive payment,public relations</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>no-till,shallow disk</t>
+  </si>
+  <si>
+    <t>soil conservation,surface water quality,groundwater quality,nutrient management,nutrient cycling,incentive payment,soil biology</t>
+  </si>
+  <si>
+    <t>Sigel,Estella</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>soil conservation,nutrient management,erosion</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>hay</t>
+  </si>
+  <si>
+    <t>winter rye, orchard grass/trefoil mix</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>harvest forage then plant,hay</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>practical soil quality benefits,natural resource and environmental economics</t>
+  </si>
+  <si>
+    <t>Wheaton,Cooksville,Woodmohr,Bloomer,Sampson,Auburn</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Delmar, Sigel</t>
+  </si>
+  <si>
+    <t>row-crop planter</t>
+  </si>
+  <si>
+    <t>acres.crop</t>
+  </si>
+  <si>
+    <t>acres.cc</t>
+  </si>
+  <si>
+    <t>no-till drill,air-flow broadcast + shallow till</t>
+  </si>
+  <si>
+    <t>no-till drill,spinner broadcast,fly-on</t>
+  </si>
+  <si>
+    <t>air-flow broadcast</t>
+  </si>
+  <si>
+    <t>unknown source</t>
   </si>
 </sst>
 </file>
@@ -519,11 +576,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,11 +896,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BAB8BD-21AD-482A-9B54-FC8CF94BAA5C}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,76 +917,76 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="U1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>143</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
-        <v>26</v>
-      </c>
       <c r="Z1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -936,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>400</v>
@@ -945,7 +1003,7 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>44845</v>
@@ -954,40 +1012,40 @@
         <v>44845</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>1.5</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L2" s="3">
         <v>90</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="W2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -995,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>990</v>
@@ -1004,7 +1062,7 @@
         <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1">
         <v>44844</v>
@@ -1013,55 +1071,55 @@
         <v>44844</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="M3" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="N3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="P3">
         <v>5000</v>
       </c>
       <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" t="s">
         <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -1069,7 +1127,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>260</v>
@@ -1078,57 +1136,57 @@
         <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I4">
         <v>1.5</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L4" s="3">
         <v>60</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" t="s">
         <v>45</v>
       </c>
-      <c r="T4" t="s">
-        <v>18</v>
-      </c>
-      <c r="U4" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>49</v>
-      </c>
       <c r="Z4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -1136,13 +1194,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5">
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>44838</v>
@@ -1151,46 +1209,46 @@
         <v>44838</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I5">
         <v>1.5</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L5" s="3">
         <v>120</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="X5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Y5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="Z5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1198,7 +1256,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>900</v>
@@ -1207,7 +1265,7 @@
         <v>240</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1">
         <v>44849</v>
@@ -1216,61 +1274,61 @@
         <v>44866</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L6" s="3">
         <v>150</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="P6">
         <v>5000</v>
       </c>
       <c r="Q6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="R6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="S6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="T6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="V6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="X6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="Y6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="Z6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1278,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>180</v>
@@ -1287,7 +1345,7 @@
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>44848</v>
@@ -1296,37 +1354,37 @@
         <v>44848</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I7">
         <v>1.5</v>
       </c>
       <c r="J7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L7" s="3">
         <v>90</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="X7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="Y7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Z7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1334,7 +1392,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>200</v>
@@ -1343,7 +1401,7 @@
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1">
         <v>44866</v>
@@ -1352,55 +1410,55 @@
         <v>44866</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>168</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="S8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W8" t="s">
+        <v>92</v>
+      </c>
+      <c r="X8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y8" t="s">
         <v>45</v>
       </c>
-      <c r="T8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" t="s">
-        <v>52</v>
-      </c>
-      <c r="W8" t="s">
-        <v>101</v>
-      </c>
-      <c r="X8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>49</v>
-      </c>
       <c r="Z8" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1408,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>425</v>
@@ -1417,54 +1475,54 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I9">
         <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L9" s="3">
         <v>80</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="V9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="W9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="Y9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1472,7 +1530,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>650</v>
@@ -1481,7 +1539,7 @@
         <v>250</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1">
         <v>44835</v>
@@ -1490,49 +1548,49 @@
         <v>44849</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10">
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L10" s="3">
         <v>56</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="U10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="W10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="X10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="Y10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="Z10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -1540,7 +1598,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>600</v>
@@ -1549,7 +1607,7 @@
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F11" s="1">
         <v>44835</v>
@@ -1558,46 +1616,46 @@
         <v>44865</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I11">
         <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L11" s="3">
         <v>180</v>
       </c>
       <c r="M11" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="N11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X11" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="Y11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="Z11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -1605,7 +1663,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>80</v>
@@ -1614,7 +1672,7 @@
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F12" s="1">
         <v>44805</v>
@@ -1623,49 +1681,49 @@
         <v>44841</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I12">
         <v>8</v>
       </c>
       <c r="J12" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="K12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="M12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="O12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="V12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W12" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="X12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Y12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -1673,7 +1731,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>2800</v>
@@ -1682,7 +1740,7 @@
         <v>170</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F13" s="1">
         <v>44847</v>
@@ -1691,49 +1749,49 @@
         <v>44847</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I13">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K13" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="M13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U13" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" t="s">
+        <v>48</v>
+      </c>
+      <c r="W13" t="s">
+        <v>49</v>
+      </c>
+      <c r="X13" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y13" t="s">
         <v>45</v>
-      </c>
-      <c r="T13" t="s">
-        <v>28</v>
-      </c>
-      <c r="U13" t="s">
-        <v>18</v>
-      </c>
-      <c r="V13" t="s">
-        <v>52</v>
-      </c>
-      <c r="W13" t="s">
-        <v>54</v>
-      </c>
-      <c r="X13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -1741,7 +1799,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>1000</v>
@@ -1750,7 +1808,7 @@
         <v>900</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F14" s="1">
         <v>44788</v>
@@ -1759,49 +1817,49 @@
         <v>44880</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I14">
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="M14" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="N14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S14" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="T14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="V14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X14" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="Y14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -1809,7 +1867,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>245</v>
@@ -1818,7 +1876,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1">
         <v>44839</v>
@@ -1827,46 +1885,46 @@
         <v>44868</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I15">
         <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K15" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L15" s="3">
         <v>70</v>
       </c>
       <c r="M15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Y15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="Z15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -1874,7 +1932,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>320</v>
@@ -1883,7 +1941,7 @@
         <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1">
         <v>44809</v>
@@ -1892,52 +1950,52 @@
         <v>44856</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I16">
         <v>5</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K16" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L16" s="3">
         <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" t="s">
+        <v>25</v>
+      </c>
+      <c r="U16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" t="s">
+        <v>48</v>
+      </c>
+      <c r="W16" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y16" t="s">
         <v>45</v>
       </c>
-      <c r="T16" t="s">
-        <v>28</v>
-      </c>
-      <c r="U16" t="s">
-        <v>18</v>
-      </c>
-      <c r="V16" t="s">
-        <v>52</v>
-      </c>
-      <c r="W16" t="s">
-        <v>15</v>
-      </c>
-      <c r="X16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>49</v>
-      </c>
       <c r="Z16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -1945,7 +2003,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C17">
         <v>97</v>
@@ -1954,7 +2012,7 @@
         <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1">
         <v>44852</v>
@@ -1963,28 +2021,28 @@
         <v>44852</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I17">
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L17" s="3">
         <v>60</v>
       </c>
       <c r="M17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Z17" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -1992,7 +2050,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>300</v>
@@ -2001,7 +2059,7 @@
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1">
         <v>44835</v>
@@ -2010,40 +2068,40 @@
         <v>44849</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I18">
         <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L18" s="3">
         <v>120</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="O18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="X18" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="Y18" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -2051,7 +2109,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>130</v>
@@ -2060,7 +2118,7 @@
         <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1">
         <v>44858</v>
@@ -2069,52 +2127,52 @@
         <v>44858</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I19">
         <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K19" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L19" s="3">
         <v>90</v>
       </c>
       <c r="M19" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S19" t="s">
+        <v>41</v>
+      </c>
+      <c r="T19" t="s">
+        <v>15</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>94</v>
+      </c>
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X19" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y19" t="s">
         <v>45</v>
       </c>
-      <c r="T19" t="s">
-        <v>18</v>
-      </c>
-      <c r="U19" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" t="s">
-        <v>103</v>
-      </c>
-      <c r="W19" t="s">
-        <v>22</v>
-      </c>
-      <c r="X19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>49</v>
-      </c>
       <c r="Z19" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -2122,7 +2180,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C20">
         <v>1500</v>
@@ -2131,7 +2189,7 @@
         <v>1400</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F20" s="1">
         <v>44783</v>
@@ -2140,46 +2198,46 @@
         <v>44866</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I20">
         <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="K20" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="M20" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="N20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="O20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S20" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="T20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="U20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="V20" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="W20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X20" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -2187,7 +2245,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21">
         <v>240</v>
@@ -2196,7 +2254,7 @@
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1">
         <v>44835</v>
@@ -2205,61 +2263,61 @@
         <v>44864</v>
       </c>
       <c r="H21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L21" s="3">
         <v>56</v>
       </c>
       <c r="M21" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="N21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O21" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="P21">
         <v>4000</v>
       </c>
       <c r="Q21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="R21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="S21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T21" t="s">
+        <v>15</v>
+      </c>
+      <c r="U21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" t="s">
+        <v>48</v>
+      </c>
+      <c r="W21" t="s">
+        <v>124</v>
+      </c>
+      <c r="X21" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" t="s">
         <v>45</v>
       </c>
-      <c r="T21" t="s">
-        <v>18</v>
-      </c>
-      <c r="U21" t="s">
-        <v>18</v>
-      </c>
-      <c r="V21" t="s">
-        <v>52</v>
-      </c>
-      <c r="W21" t="s">
-        <v>134</v>
-      </c>
-      <c r="X21" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>49</v>
-      </c>
       <c r="Z21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -2267,7 +2325,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>112</v>
@@ -2276,7 +2334,7 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1">
         <v>44839</v>
@@ -2285,49 +2343,49 @@
         <v>44839</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22">
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K22" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L22" s="3">
         <v>56</v>
       </c>
       <c r="M22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="U22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="V22" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="W22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X22" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="Y22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -2335,7 +2393,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -2344,7 +2402,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F23" s="1">
         <v>44866</v>
@@ -2353,43 +2411,43 @@
         <v>44866</v>
       </c>
       <c r="H23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I23">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K23" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L23" s="3">
         <v>20</v>
       </c>
       <c r="M23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="W23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X23" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="Z23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -2397,7 +2455,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>85</v>
@@ -2406,7 +2464,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1">
         <v>44854</v>
@@ -2415,46 +2473,46 @@
         <v>44854</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I24">
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K24" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L24" s="3">
         <v>100</v>
       </c>
       <c r="M24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S24" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="V24" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="W24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X24" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="Y24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -2462,7 +2520,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>94</v>
@@ -2471,7 +2529,7 @@
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F25" s="1">
         <v>44870</v>
@@ -2480,52 +2538,52 @@
         <v>44870</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I25">
         <v>1.5</v>
       </c>
       <c r="J25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L25" s="3">
         <v>60</v>
       </c>
       <c r="M25" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="N25" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="O25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S25" t="s">
+        <v>41</v>
+      </c>
+      <c r="T25" t="s">
+        <v>15</v>
+      </c>
+      <c r="U25" t="s">
+        <v>15</v>
+      </c>
+      <c r="V25" t="s">
+        <v>80</v>
+      </c>
+      <c r="W25" t="s">
+        <v>49</v>
+      </c>
+      <c r="X25" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y25" t="s">
         <v>45</v>
       </c>
-      <c r="T25" t="s">
-        <v>18</v>
-      </c>
-      <c r="U25" t="s">
-        <v>18</v>
-      </c>
-      <c r="V25" t="s">
-        <v>89</v>
-      </c>
-      <c r="W25" t="s">
-        <v>54</v>
-      </c>
-      <c r="X25" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>49</v>
-      </c>
       <c r="Z25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -2533,7 +2591,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -2542,7 +2600,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F26" s="1">
         <v>44802</v>
@@ -2551,43 +2609,587 @@
         <v>44830</v>
       </c>
       <c r="H26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I26">
         <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L26" s="3">
         <v>300</v>
       </c>
       <c r="M26" t="s">
+        <v>64</v>
+      </c>
+      <c r="N26" t="s">
+        <v>65</v>
+      </c>
+      <c r="O26" t="s">
+        <v>15</v>
+      </c>
+      <c r="S26" t="s">
+        <v>41</v>
+      </c>
+      <c r="V26" t="s">
+        <v>48</v>
+      </c>
+      <c r="W26" t="s">
+        <v>12</v>
+      </c>
+      <c r="X26" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>280</v>
+      </c>
+      <c r="D27">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1">
+        <v>44846</v>
+      </c>
+      <c r="G27" s="1">
+        <v>44846</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27">
+        <v>2.5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" t="s">
+        <v>134</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M27" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27">
+        <v>6000</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>34</v>
+      </c>
+      <c r="R27" t="s">
+        <v>32</v>
+      </c>
+      <c r="S27" t="s">
+        <v>41</v>
+      </c>
+      <c r="T27" t="s">
+        <v>15</v>
+      </c>
+      <c r="U27" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27" t="s">
+        <v>80</v>
+      </c>
+      <c r="W27" t="s">
+        <v>12</v>
+      </c>
+      <c r="X27" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1">
+        <v>44846</v>
+      </c>
+      <c r="G28" s="1">
+        <v>44846</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M28" t="s">
+        <v>57</v>
+      </c>
+      <c r="N28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28" t="s">
+        <v>41</v>
+      </c>
+      <c r="T28" t="s">
+        <v>25</v>
+      </c>
+      <c r="U28" t="s">
+        <v>25</v>
+      </c>
+      <c r="V28" t="s">
+        <v>48</v>
+      </c>
+      <c r="W28" t="s">
+        <v>12</v>
+      </c>
+      <c r="X28" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29">
+        <v>348</v>
+      </c>
+      <c r="D29">
+        <v>348</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="1">
+        <v>44854</v>
+      </c>
+      <c r="G29" s="1">
+        <v>44888</v>
+      </c>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M29" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29" t="s">
+        <v>147</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+      <c r="S29" t="s">
+        <v>41</v>
+      </c>
+      <c r="T29" t="s">
+        <v>15</v>
+      </c>
+      <c r="U29" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" t="s">
+        <v>48</v>
+      </c>
+      <c r="W29" t="s">
+        <v>19</v>
+      </c>
+      <c r="X29" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30">
+        <v>295</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" t="s">
+        <v>134</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M30" t="s">
+        <v>57</v>
+      </c>
+      <c r="N30" t="s">
+        <v>65</v>
+      </c>
+      <c r="O30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" t="s">
+        <v>41</v>
+      </c>
+      <c r="T30" t="s">
+        <v>25</v>
+      </c>
+      <c r="U30" t="s">
+        <v>25</v>
+      </c>
+      <c r="V30" t="s">
+        <v>48</v>
+      </c>
+      <c r="W30" t="s">
+        <v>19</v>
+      </c>
+      <c r="X30" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31">
+        <v>34</v>
+      </c>
+      <c r="D31">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44830</v>
+      </c>
+      <c r="G31" s="1">
+        <v>44831</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>154</v>
+      </c>
+      <c r="K31" t="s">
+        <v>134</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" t="s">
+        <v>35</v>
+      </c>
+      <c r="V31" t="s">
+        <v>156</v>
+      </c>
+      <c r="W31" t="s">
+        <v>153</v>
+      </c>
+      <c r="X31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="1">
+        <v>44856</v>
+      </c>
+      <c r="G32" s="1">
+        <v>44857</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32">
+        <v>1.5</v>
+      </c>
+      <c r="J32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>134</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" t="s">
+        <v>15</v>
+      </c>
+      <c r="S32" t="s">
+        <v>41</v>
+      </c>
+      <c r="T32" t="s">
+        <v>15</v>
+      </c>
+      <c r="U32" t="s">
+        <v>15</v>
+      </c>
+      <c r="V32" t="s">
+        <v>48</v>
+      </c>
+      <c r="W32" t="s">
+        <v>19</v>
+      </c>
+      <c r="X32" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33">
+        <v>3000</v>
+      </c>
+      <c r="D33">
+        <v>1350</v>
+      </c>
+      <c r="E33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="1">
+        <v>44840</v>
+      </c>
+      <c r="G33" s="1">
+        <v>44866</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" t="s">
+        <v>134</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M33" t="s">
+        <v>27</v>
+      </c>
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S33" t="s">
+        <v>35</v>
+      </c>
+      <c r="V33" t="s">
+        <v>48</v>
+      </c>
+      <c r="W33" t="s">
+        <v>81</v>
+      </c>
+      <c r="X33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34">
+        <v>400</v>
+      </c>
+      <c r="D34">
+        <v>200</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="1">
+        <v>44849</v>
+      </c>
+      <c r="G34" s="1">
+        <v>44855</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>134</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M34" t="s">
+        <v>162</v>
+      </c>
+      <c r="N34" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" t="s">
+        <v>15</v>
+      </c>
+      <c r="S34" t="s">
+        <v>41</v>
+      </c>
+      <c r="T34" t="s">
+        <v>25</v>
+      </c>
+      <c r="U34" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" t="s">
+        <v>48</v>
+      </c>
+      <c r="W34" t="s">
+        <v>19</v>
+      </c>
+      <c r="X34" t="s">
         <v>71</v>
       </c>
-      <c r="N26" t="s">
-        <v>72</v>
-      </c>
-      <c r="O26" t="s">
-        <v>18</v>
-      </c>
-      <c r="S26" t="s">
-        <v>45</v>
-      </c>
-      <c r="V26" t="s">
-        <v>52</v>
-      </c>
-      <c r="W26" t="s">
-        <v>15</v>
-      </c>
-      <c r="X26" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>92</v>
+      <c r="Y34" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more survey responses and updated figures
</commit_message>
<xml_diff>
--- a/2022CCSurvey_1.xlsx
+++ b/2022CCSurvey_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/kolby_grint_usda_gov/Documents/Documents/R Vizualizations and Data/Chippewa-County-Cover-Crop-Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6153BD4-DDF6-4855-9B63-F51C42F3EDB2}"/>
+  <xr:revisionPtr revIDLastSave="645" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D378D399-9517-40FB-8D7A-4590ACBF932A}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{3ABCB6C5-5AC4-4763-96A0-86D19504B3A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3ABCB6C5-5AC4-4763-96A0-86D19504B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="174">
   <si>
     <t>respondent</t>
   </si>
@@ -255,9 +255,6 @@
     <t>no-till,shallow vertical</t>
   </si>
   <si>
-    <t>winter rye, winter wheat</t>
-  </si>
-  <si>
     <t>soybean,corn silage</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>soybean,potatoes,sweet corn,tomatoes</t>
   </si>
   <si>
-    <t>winter rye,oats</t>
-  </si>
-  <si>
     <t>shallow vertical,shallow disk</t>
   </si>
   <si>
@@ -357,9 +351,6 @@
     <t>soybean,corn grain,oats,rye,snap beans</t>
   </si>
   <si>
-    <t>winter rye,oats,clover,peas,buckwheat,turnips</t>
-  </si>
-  <si>
     <t>bin run,common variety</t>
   </si>
   <si>
@@ -498,9 +489,6 @@
     <t>hay</t>
   </si>
   <si>
-    <t>winter rye, orchard grass/trefoil mix</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
@@ -519,9 +507,6 @@
     <t>56</t>
   </si>
   <si>
-    <t>Delmar, Sigel</t>
-  </si>
-  <si>
     <t>row-crop planter</t>
   </si>
   <si>
@@ -541,6 +526,36 @@
   </si>
   <si>
     <t>unknown source</t>
+  </si>
+  <si>
+    <t>Delmar,Sigel</t>
+  </si>
+  <si>
+    <t>Bloomer</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>soil conservation,surface water quality</t>
+  </si>
+  <si>
+    <t>the work</t>
+  </si>
+  <si>
+    <t>soybean,snap beans</t>
+  </si>
+  <si>
+    <t>winter rye,oat</t>
+  </si>
+  <si>
+    <t>178,80</t>
+  </si>
+  <si>
+    <t>winter rye,orchard grass/trefoil mix</t>
+  </si>
+  <si>
+    <t>winter rye,oat,clover,peas,buckwheat,turnips</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,11 +911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BAB8BD-21AD-482A-9B54-FC8CF94BAA5C}">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -941,7 +956,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>10</v>
@@ -986,7 +1001,7 @@
         <v>23</v>
       </c>
       <c r="Z1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -1021,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L2" s="3">
         <v>90</v>
@@ -1062,7 +1077,7 @@
         <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1">
         <v>44844</v>
@@ -1077,16 +1092,16 @@
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="N3" t="s">
         <v>72</v>
@@ -1113,7 +1128,7 @@
         <v>19</v>
       </c>
       <c r="X3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y3" t="s">
         <v>45</v>
@@ -1150,7 +1165,7 @@
         <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L4" s="3">
         <v>60</v>
@@ -1180,13 +1195,13 @@
         <v>19</v>
       </c>
       <c r="X4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y4" t="s">
         <v>45</v>
       </c>
       <c r="Z4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -1218,7 +1233,7 @@
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L5" s="3">
         <v>120</v>
@@ -1265,7 +1280,7 @@
         <v>240</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1">
         <v>44849</v>
@@ -1274,7 +1289,7 @@
         <v>44866</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -1283,7 +1298,7 @@
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L6" s="3">
         <v>150</v>
@@ -1307,7 +1322,7 @@
         <v>32</v>
       </c>
       <c r="S6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T6" t="s">
         <v>25</v>
@@ -1316,19 +1331,19 @@
         <v>15</v>
       </c>
       <c r="V6" t="s">
+        <v>79</v>
+      </c>
+      <c r="W6" t="s">
         <v>80</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>81</v>
-      </c>
-      <c r="X6" t="s">
-        <v>82</v>
       </c>
       <c r="Y6" t="s">
         <v>45</v>
       </c>
       <c r="Z6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1363,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L7" s="3">
         <v>90</v>
@@ -1378,13 +1393,13 @@
         <v>15</v>
       </c>
       <c r="X7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y7" t="s">
         <v>56</v>
       </c>
       <c r="Z7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1401,7 +1416,7 @@
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1">
         <v>44866</v>
@@ -1416,13 +1431,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="K8" t="s">
-        <v>135</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="M8" t="s">
         <v>57</v>
@@ -1431,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="O8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="R8" t="s">
         <v>58</v>
@@ -1449,7 +1464,7 @@
         <v>48</v>
       </c>
       <c r="W8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X8" t="s">
         <v>71</v>
@@ -1458,7 +1473,7 @@
         <v>45</v>
       </c>
       <c r="Z8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1475,7 +1490,7 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1489,7 +1504,7 @@
         <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L9" s="3">
         <v>80</v>
@@ -1513,13 +1528,13 @@
         <v>25</v>
       </c>
       <c r="V9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W9" t="s">
         <v>19</v>
       </c>
       <c r="X9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y9" t="s">
         <v>60</v>
@@ -1539,7 +1554,7 @@
         <v>250</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1">
         <v>44835</v>
@@ -1557,7 +1572,7 @@
         <v>9</v>
       </c>
       <c r="K10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L10" s="3">
         <v>56</v>
@@ -1581,16 +1596,16 @@
         <v>25</v>
       </c>
       <c r="W10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y10" t="s">
         <v>61</v>
       </c>
       <c r="Z10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -1607,7 +1622,7 @@
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" s="1">
         <v>44835</v>
@@ -1625,13 +1640,13 @@
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L11" s="3">
         <v>180</v>
       </c>
       <c r="M11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="N11" t="s">
         <v>13</v>
@@ -1672,7 +1687,7 @@
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F12" s="1">
         <v>44805</v>
@@ -1687,19 +1702,19 @@
         <v>8</v>
       </c>
       <c r="J12" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="K12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="M12" t="s">
         <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
         <v>15</v>
@@ -1717,7 +1732,7 @@
         <v>48</v>
       </c>
       <c r="W12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X12" t="s">
         <v>21</v>
@@ -1731,7 +1746,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13">
         <v>2800</v>
@@ -1740,7 +1755,7 @@
         <v>170</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F13" s="1">
         <v>44847</v>
@@ -1758,10 +1773,10 @@
         <v>9</v>
       </c>
       <c r="K13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M13" t="s">
         <v>64</v>
@@ -1788,7 +1803,7 @@
         <v>49</v>
       </c>
       <c r="X13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Y13" t="s">
         <v>45</v>
@@ -1808,7 +1823,7 @@
         <v>900</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>44788</v>
@@ -1823,16 +1838,16 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="K14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="N14" t="s">
         <v>13</v>
@@ -1841,7 +1856,7 @@
         <v>15</v>
       </c>
       <c r="S14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="T14" t="s">
         <v>25</v>
@@ -1856,7 +1871,7 @@
         <v>19</v>
       </c>
       <c r="X14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Y14" t="s">
         <v>45</v>
@@ -1894,7 +1909,7 @@
         <v>9</v>
       </c>
       <c r="K15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L15" s="3">
         <v>70</v>
@@ -1959,7 +1974,7 @@
         <v>9</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L16" s="3">
         <v>60</v>
@@ -2003,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>97</v>
@@ -2030,7 +2045,7 @@
         <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L17" s="3">
         <v>60</v>
@@ -2042,7 +2057,7 @@
         <v>13</v>
       </c>
       <c r="Z17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -2077,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L18" s="3">
         <v>120</v>
@@ -2098,7 +2113,7 @@
         <v>54</v>
       </c>
       <c r="X18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y18" t="s">
         <v>67</v>
@@ -2109,7 +2124,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>130</v>
@@ -2136,7 +2151,7 @@
         <v>9</v>
       </c>
       <c r="K19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L19" s="3">
         <v>90</v>
@@ -2160,19 +2175,19 @@
         <v>15</v>
       </c>
       <c r="V19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W19" t="s">
         <v>19</v>
       </c>
       <c r="X19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Y19" t="s">
         <v>45</v>
       </c>
       <c r="Z19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -2180,7 +2195,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C20">
         <v>1500</v>
@@ -2189,7 +2204,7 @@
         <v>1400</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F20" s="1">
         <v>44783</v>
@@ -2204,16 +2219,16 @@
         <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N20" t="s">
         <v>65</v>
@@ -2222,7 +2237,7 @@
         <v>15</v>
       </c>
       <c r="S20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="T20" t="s">
         <v>25</v>
@@ -2231,13 +2246,13 @@
         <v>25</v>
       </c>
       <c r="V20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="W20" t="s">
         <v>12</v>
       </c>
       <c r="X20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -2254,7 +2269,7 @@
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="1">
         <v>44835</v>
@@ -2272,7 +2287,7 @@
         <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L21" s="3">
         <v>56</v>
@@ -2308,7 +2323,7 @@
         <v>48</v>
       </c>
       <c r="W21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="X21" t="s">
         <v>22</v>
@@ -2352,7 +2367,7 @@
         <v>9</v>
       </c>
       <c r="K22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L22" s="3">
         <v>56</v>
@@ -2382,7 +2397,7 @@
         <v>12</v>
       </c>
       <c r="X22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y22" t="s">
         <v>69</v>
@@ -2420,7 +2435,7 @@
         <v>9</v>
       </c>
       <c r="K23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L23" s="3">
         <v>20</v>
@@ -2444,10 +2459,10 @@
         <v>12</v>
       </c>
       <c r="X23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -2482,7 +2497,7 @@
         <v>9</v>
       </c>
       <c r="K24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L24" s="3">
         <v>100</v>
@@ -2500,13 +2515,13 @@
         <v>35</v>
       </c>
       <c r="V24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="W24" t="s">
         <v>19</v>
       </c>
       <c r="X24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Y24" t="s">
         <v>45</v>
@@ -2529,7 +2544,7 @@
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="1">
         <v>44870</v>
@@ -2547,16 +2562,16 @@
         <v>9</v>
       </c>
       <c r="K25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L25" s="3">
         <v>60</v>
       </c>
       <c r="M25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O25" t="s">
         <v>15</v>
@@ -2571,13 +2586,13 @@
         <v>15</v>
       </c>
       <c r="V25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W25" t="s">
         <v>49</v>
       </c>
       <c r="X25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Y25" t="s">
         <v>45</v>
@@ -2618,7 +2633,7 @@
         <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L26" s="3">
         <v>300</v>
@@ -2642,10 +2657,10 @@
         <v>12</v>
       </c>
       <c r="X26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -2680,10 +2695,10 @@
         <v>9</v>
       </c>
       <c r="K27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M27" t="s">
         <v>55</v>
@@ -2713,16 +2728,16 @@
         <v>15</v>
       </c>
       <c r="V27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W27" t="s">
         <v>12</v>
       </c>
       <c r="X27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Y27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -2757,10 +2772,10 @@
         <v>9</v>
       </c>
       <c r="K28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M28" t="s">
         <v>57</v>
@@ -2787,10 +2802,10 @@
         <v>12</v>
       </c>
       <c r="X28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Y28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -2807,7 +2822,7 @@
         <v>348</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" s="1">
         <v>44854</v>
@@ -2825,16 +2840,16 @@
         <v>9</v>
       </c>
       <c r="K29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M29" t="s">
         <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O29" t="s">
         <v>15</v>
@@ -2855,10 +2870,10 @@
         <v>19</v>
       </c>
       <c r="X29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="Y29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -2866,7 +2881,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C30">
         <v>295</v>
@@ -2887,10 +2902,10 @@
         <v>9</v>
       </c>
       <c r="K30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M30" t="s">
         <v>57</v>
@@ -2917,7 +2932,7 @@
         <v>19</v>
       </c>
       <c r="X30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="Y30" t="s">
         <v>45</v>
@@ -2931,7 +2946,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31">
         <v>34</v>
@@ -2940,7 +2955,7 @@
         <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F31" s="1">
         <v>44830</v>
@@ -2955,13 +2970,13 @@
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="K31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M31" t="s">
         <v>27</v>
@@ -2976,16 +2991,16 @@
         <v>35</v>
       </c>
       <c r="V31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="W31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="X31" t="s">
         <v>21</v>
       </c>
       <c r="Y31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -3020,10 +3035,10 @@
         <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="M32" t="s">
         <v>27</v>
@@ -3050,13 +3065,13 @@
         <v>19</v>
       </c>
       <c r="X32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Z32" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
@@ -3064,7 +3079,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C33">
         <v>3000</v>
@@ -3073,7 +3088,7 @@
         <v>1350</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1">
         <v>44840</v>
@@ -3091,10 +3106,10 @@
         <v>9</v>
       </c>
       <c r="K33" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M33" t="s">
         <v>27</v>
@@ -3112,16 +3127,16 @@
         <v>48</v>
       </c>
       <c r="W33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X33" t="s">
         <v>21</v>
       </c>
       <c r="Y33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Z33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
@@ -3129,7 +3144,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C34">
         <v>400</v>
@@ -3150,19 +3165,19 @@
         <v>25</v>
       </c>
       <c r="I34" s="4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="J34" t="s">
         <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L34" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M34" t="s">
         <v>157</v>
-      </c>
-      <c r="M34" t="s">
-        <v>162</v>
       </c>
       <c r="N34" t="s">
         <v>13</v>
@@ -3189,7 +3204,220 @@
         <v>71</v>
       </c>
       <c r="Y34" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35">
+        <v>1535</v>
+      </c>
+      <c r="D35">
+        <v>517</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44872</v>
+      </c>
+      <c r="G35" s="1">
+        <v>44880</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" t="s">
+        <v>131</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M35" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" t="s">
+        <v>29</v>
+      </c>
+      <c r="O35" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" t="s">
+        <v>41</v>
+      </c>
+      <c r="T35" t="s">
+        <v>15</v>
+      </c>
+      <c r="U35" t="s">
+        <v>15</v>
+      </c>
+      <c r="V35" t="s">
+        <v>48</v>
+      </c>
+      <c r="W35" t="s">
+        <v>49</v>
+      </c>
+      <c r="X35" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36">
+        <v>1780</v>
+      </c>
+      <c r="D36">
+        <v>475</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44866</v>
+      </c>
+      <c r="G36" s="1">
+        <v>44884</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36">
+        <v>0.5</v>
+      </c>
+      <c r="J36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" t="s">
+        <v>131</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M36" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" t="s">
+        <v>29</v>
+      </c>
+      <c r="O36" t="s">
+        <v>15</v>
+      </c>
+      <c r="S36" t="s">
+        <v>41</v>
+      </c>
+      <c r="T36" t="s">
+        <v>15</v>
+      </c>
+      <c r="U36" t="s">
+        <v>15</v>
+      </c>
+      <c r="V36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W36" t="s">
+        <v>49</v>
+      </c>
+      <c r="X36" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37">
+        <v>4175</v>
+      </c>
+      <c r="D37">
+        <v>875</v>
+      </c>
+      <c r="E37" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="1">
+        <v>44852</v>
+      </c>
+      <c r="G37" s="1">
+        <v>44885</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37">
+        <v>1.5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>170</v>
+      </c>
+      <c r="K37" t="s">
+        <v>131</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M37" t="s">
+        <v>64</v>
+      </c>
+      <c r="N37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O37" t="s">
+        <v>15</v>
+      </c>
+      <c r="S37" t="s">
+        <v>41</v>
+      </c>
+      <c r="T37" t="s">
+        <v>15</v>
+      </c>
+      <c r="U37" t="s">
+        <v>15</v>
+      </c>
+      <c r="V37" t="s">
+        <v>48</v>
+      </c>
+      <c r="W37" t="s">
+        <v>49</v>
+      </c>
+      <c r="X37" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added another survey to the dataset.
</commit_message>
<xml_diff>
--- a/2022CCSurvey_1.xlsx
+++ b/2022CCSurvey_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/kolby_grint_usda_gov/Documents/Documents/R Vizualizations and Data/Chippewa-County-Cover-Crop-Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="645" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D378D399-9517-40FB-8D7A-4590ACBF932A}"/>
+  <xr:revisionPtr revIDLastSave="677" documentId="8_{13D86688-3ADA-4B0D-9533-50E5C8D707BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFFC581A-E770-4288-83CC-5E5F3E80EEC3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3ABCB6C5-5AC4-4763-96A0-86D19504B3A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="181">
   <si>
     <t>respondent</t>
   </si>
@@ -556,6 +556,27 @@
   </si>
   <si>
     <t>winter rye,oat,clover,peas,buckwheat,turnips</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>solid</t>
+  </si>
+  <si>
+    <t>before,after</t>
+  </si>
+  <si>
+    <t>24,24</t>
+  </si>
+  <si>
+    <t>solid,solid</t>
+  </si>
+  <si>
+    <t>soil conservation,nutrient management,manure management,nutrient cycling,incentive payment,public relations</t>
+  </si>
+  <si>
+    <t>termination economics</t>
   </si>
 </sst>
 </file>
@@ -911,11 +932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BAB8BD-21AD-482A-9B54-FC8CF94BAA5C}">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3420,6 +3441,86 @@
         <v>96</v>
       </c>
     </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38">
+        <v>850</v>
+      </c>
+      <c r="D38">
+        <v>225</v>
+      </c>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44849</v>
+      </c>
+      <c r="G38" s="1">
+        <v>44873</v>
+      </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" t="s">
+        <v>131</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M38" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" t="s">
+        <v>13</v>
+      </c>
+      <c r="O38" t="s">
+        <v>175</v>
+      </c>
+      <c r="P38" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>178</v>
+      </c>
+      <c r="R38" t="s">
+        <v>176</v>
+      </c>
+      <c r="S38" t="s">
+        <v>41</v>
+      </c>
+      <c r="T38" t="s">
+        <v>25</v>
+      </c>
+      <c r="U38" t="s">
+        <v>25</v>
+      </c>
+      <c r="V38" t="s">
+        <v>93</v>
+      </c>
+      <c r="W38" t="s">
+        <v>19</v>
+      </c>
+      <c r="X38" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>